<commit_message>
updated and reformatted tables
</commit_message>
<xml_diff>
--- a/magic_item_tables.xlsx
+++ b/magic_item_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9CDDB5-340D-4460-9E31-CF37697087BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B05EB3-57BD-47E0-B8EE-D498DC34459D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="8" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27620" yWindow="3940" windowWidth="20820" windowHeight="17410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table A" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,8 @@
     <sheet name="Table E" sheetId="5" r:id="rId5"/>
     <sheet name="Table F" sheetId="6" r:id="rId6"/>
     <sheet name="Table G" sheetId="7" r:id="rId7"/>
-    <sheet name="Figureine of Wondrous Power" sheetId="8" r:id="rId8"/>
-    <sheet name="Table H" sheetId="11" r:id="rId9"/>
-    <sheet name="Table I" sheetId="9" r:id="rId10"/>
-    <sheet name="Magic Armor" sheetId="10" r:id="rId11"/>
-    <sheet name="Armor" sheetId="12" r:id="rId12"/>
-    <sheet name="Weapons" sheetId="13" r:id="rId13"/>
-    <sheet name="Ammunition" sheetId="14" r:id="rId14"/>
-    <sheet name="Gems" sheetId="15" r:id="rId15"/>
-    <sheet name="Art Objects" sheetId="16" r:id="rId16"/>
+    <sheet name="Table H" sheetId="11" r:id="rId8"/>
+    <sheet name="Table I" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -40,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="361">
   <si>
     <t>Potion of Healing</t>
   </si>
@@ -750,27 +743,6 @@
     <t>Wings of flying</t>
   </si>
   <si>
-    <t>Onyx dog</t>
-  </si>
-  <si>
-    <t>Serpentine owl</t>
-  </si>
-  <si>
-    <t>Bronze griffon</t>
-  </si>
-  <si>
-    <t>Ebony fly</t>
-  </si>
-  <si>
-    <t>Golden lions</t>
-  </si>
-  <si>
-    <t>Ivory goats</t>
-  </si>
-  <si>
-    <t>Marble elephant</t>
-  </si>
-  <si>
     <t>Defender</t>
   </si>
   <si>
@@ -852,27 +824,6 @@
     <t>Magic armor (roll 1d12)</t>
   </si>
   <si>
-    <t>Armor, +2 plate</t>
-  </si>
-  <si>
-    <t>Armor, +3 studded leather</t>
-  </si>
-  <si>
-    <t>Armor, +3 breastplate</t>
-  </si>
-  <si>
-    <t>Armor, +3 splint</t>
-  </si>
-  <si>
-    <t>Armor, +3 half plate</t>
-  </si>
-  <si>
-    <t>Armor, +3 plate</t>
-  </si>
-  <si>
-    <t>Armor, +2 half plate</t>
-  </si>
-  <si>
     <t>Apparatus of Kwalish</t>
   </si>
   <si>
@@ -1152,168 +1103,6 @@
     <t>Tome of understanding</t>
   </si>
   <si>
-    <t>Plate</t>
-  </si>
-  <si>
-    <t>Splint</t>
-  </si>
-  <si>
-    <t>Chain mail</t>
-  </si>
-  <si>
-    <t>Half plate</t>
-  </si>
-  <si>
-    <t>Breastplate</t>
-  </si>
-  <si>
-    <t>Scale mail</t>
-  </si>
-  <si>
-    <t>Chain shirt</t>
-  </si>
-  <si>
-    <t>Hide</t>
-  </si>
-  <si>
-    <t>Studded leather</t>
-  </si>
-  <si>
-    <t>Leather</t>
-  </si>
-  <si>
-    <t> Padded</t>
-  </si>
-  <si>
-    <t>Club</t>
-  </si>
-  <si>
-    <t>Dagger</t>
-  </si>
-  <si>
-    <t>Greatclub</t>
-  </si>
-  <si>
-    <t>Net</t>
-  </si>
-  <si>
-    <t>Longbow</t>
-  </si>
-  <si>
-    <t>Crossbow, heavy</t>
-  </si>
-  <si>
-    <t>Crossbow, hand</t>
-  </si>
-  <si>
-    <t>Blowgun</t>
-  </si>
-  <si>
-    <t>Whip</t>
-  </si>
-  <si>
-    <t>Warhammer</t>
-  </si>
-  <si>
-    <t>War pick</t>
-  </si>
-  <si>
-    <t>Trident</t>
-  </si>
-  <si>
-    <t>Shortsword</t>
-  </si>
-  <si>
-    <t>Scimitar</t>
-  </si>
-  <si>
-    <t>Rapier</t>
-  </si>
-  <si>
-    <t>Pike</t>
-  </si>
-  <si>
-    <t>Morningstar</t>
-  </si>
-  <si>
-    <t>Maul</t>
-  </si>
-  <si>
-    <t>Longsword</t>
-  </si>
-  <si>
-    <t>Lance</t>
-  </si>
-  <si>
-    <t>Halberd</t>
-  </si>
-  <si>
-    <t>Greatsword</t>
-  </si>
-  <si>
-    <t>Greataxe</t>
-  </si>
-  <si>
-    <t>Handaxe</t>
-  </si>
-  <si>
-    <t>Light hammer</t>
-  </si>
-  <si>
-    <t>Quarterstaff</t>
-  </si>
-  <si>
-    <t>Sickle</t>
-  </si>
-  <si>
-    <t>Spear</t>
-  </si>
-  <si>
-    <t>Crossbow, light</t>
-  </si>
-  <si>
-    <t>Dart</t>
-  </si>
-  <si>
-    <t>Shortbow</t>
-  </si>
-  <si>
-    <t>Battleaxe</t>
-  </si>
-  <si>
-    <t>Flail</t>
-  </si>
-  <si>
-    <t>Glaive</t>
-  </si>
-  <si>
-    <t>Sling</t>
-  </si>
-  <si>
-    <t>Mace</t>
-  </si>
-  <si>
-    <t>Javelin</t>
-  </si>
-  <si>
-    <t>Arrows (20)</t>
-  </si>
-  <si>
-    <t>Blowgun needles (50)</t>
-  </si>
-  <si>
-    <t>Crossbow bolts (20)</t>
-  </si>
-  <si>
-    <t>Sling bullets (20)</t>
-  </si>
-  <si>
-    <t>Hand Axe</t>
-  </si>
-  <si>
-    <t>Light Hammer</t>
-  </si>
-  <si>
     <t>Shield, +1</t>
   </si>
   <si>
@@ -1327,332 +1116,16 @@
   </si>
   <si>
     <t>Staff of the Magi</t>
-  </si>
-  <si>
-    <t>–</t>
-  </si>
-  <si>
-    <t>Ruby (transparent clear red to deep crimson)</t>
-  </si>
-  <si>
-    <t>Star ruby (translucent ruby with white star-shaped center)</t>
-  </si>
-  <si>
-    <t>Topaz (transparent golden yellow)</t>
-  </si>
-  <si>
-    <t>Zircon (transparent pale blue-green)</t>
-  </si>
-  <si>
-    <t>Turquoise (opaque light blue-green)</t>
-  </si>
-  <si>
-    <t>Jacinth (transparent fiery orange)</t>
-  </si>
-  <si>
-    <t>Fire opal (translucent fiery red)</t>
-  </si>
-  <si>
-    <t>Peridot (transparent rich olive green)</t>
-  </si>
-  <si>
-    <t>Star rose quartz (translucent rosy stone with white star-shaped center)</t>
-  </si>
-  <si>
-    <t>Tiger eye (translucent brown with golden center)</t>
-  </si>
-  <si>
-    <t>Diamond (transparent blue-white, canary, pink, brown, or blue)</t>
-  </si>
-  <si>
-    <t>Emerald (transparent deep bright green)</t>
-  </si>
-  <si>
-    <t>Blue spinel (transparent deep blue)</t>
-  </si>
-  <si>
-    <t>Sardonyx (opaque bands of red and white)</t>
-  </si>
-  <si>
-    <t>Rhodochrosite (opaque light pink)</t>
-  </si>
-  <si>
-    <t>Black sapphire (translucent lustrous black with glowing highlights)</t>
-  </si>
-  <si>
-    <t>Blue sapphire (transparent blue-white to medium blue)</t>
-  </si>
-  <si>
-    <t>Black pearl (opaque pure black)</t>
-  </si>
-  <si>
-    <t>Quartz (transparent white, smoky gray, or yellow)</t>
-  </si>
-  <si>
-    <t>Obsidian (opaque black)</t>
-  </si>
-  <si>
-    <t>Yellow sapphire (transparent fiery yellow or yellow green)</t>
-  </si>
-  <si>
-    <t>Aquamarine (transparent pale blue-green)</t>
-  </si>
-  <si>
-    <t>Onyx (opaque bands of black and white, or pure black or white)</t>
-  </si>
-  <si>
-    <t>Moss agate (translucent pink or yellow-white with mossy gray or green markings)</t>
-  </si>
-  <si>
-    <t>Star sapphire (translucent blue sapphire with white star-shaped center)</t>
-  </si>
-  <si>
-    <t>Alexandrite (transparent dark green)</t>
-  </si>
-  <si>
-    <t>Moonstone (translucent white with pale blue glow)</t>
-  </si>
-  <si>
-    <t>Malachite (opaque striated light and dark green)</t>
-  </si>
-  <si>
-    <t>Jasper (opaque blue, black, or brown)</t>
-  </si>
-  <si>
-    <t>Lapis lazuli (opaque light and dark blue with yellow flecks)</t>
-  </si>
-  <si>
-    <t>Opal (translucent pale blue with green and golden mottling)</t>
-  </si>
-  <si>
-    <t>Citrine (transparent pale yellow-brown)</t>
-  </si>
-  <si>
-    <t>Hematite (opaque gray-black)</t>
-  </si>
-  <si>
-    <t>Chrysoprase (translucent green)</t>
-  </si>
-  <si>
-    <t>Eye agate (translucent circles of gray, white, brown, blue, or green)</t>
-  </si>
-  <si>
-    <t>Chalcedony (opaque white)</t>
-  </si>
-  <si>
-    <t>Blue quartz (transparent pale blue)</t>
-  </si>
-  <si>
-    <t>Carnelian (opaque orange to red-brown)</t>
-  </si>
-  <si>
-    <t>Banded agate (translucent striped brown, blue, white, or red)</t>
-  </si>
-  <si>
-    <t>Black opal (translucent dark green with black mottling and golden flecks)</t>
-  </si>
-  <si>
-    <t>Bloodstone (opaque dark gray with red flecks)</t>
-  </si>
-  <si>
-    <t>Azurite (opaque mottled deep blue)</t>
-  </si>
-  <si>
-    <t>5000 GP</t>
-  </si>
-  <si>
-    <t>1000 GP</t>
-  </si>
-  <si>
-    <t>500 GP</t>
-  </si>
-  <si>
-    <t>50 GP</t>
-  </si>
-  <si>
-    <t>10 GP</t>
-  </si>
-  <si>
-    <t>A necklace string of small pink pearls</t>
-  </si>
-  <si>
-    <t>Painted gold war mask</t>
-  </si>
-  <si>
-    <t>Gold bird cage with electrum filigree</t>
-  </si>
-  <si>
-    <t>Gold locket with a painted portrait inside</t>
-  </si>
-  <si>
-    <t>Eye patch with a mock eye set in blue sapphire andmoonstone</t>
-  </si>
-  <si>
-    <t>Obsidian statuette with gold fittings and inlay</t>
-  </si>
-  <si>
-    <t>Box of turquoise animal figurines</t>
-  </si>
-  <si>
-    <t>Embroidered silk handkerchief</t>
-  </si>
-  <si>
-    <t>Bejeweled ivory drinking horn with gold filigree</t>
-  </si>
-  <si>
-    <t>Gold circlet set with four aquamarines</t>
-  </si>
-  <si>
-    <t>Silver and gold brooch</t>
-  </si>
-  <si>
-    <t>Brass mug with jade inlay</t>
-  </si>
-  <si>
-    <t>Small mirror set in a painted wooden frame</t>
-  </si>
-  <si>
-    <t>Jade game board with solid gold playing pieces</t>
-  </si>
-  <si>
-    <t>Gold music box</t>
-  </si>
-  <si>
-    <t>Ceremonial electrum dagger with a black pearl in the pommel</t>
-  </si>
-  <si>
-    <t>Large well-made tapestry</t>
-  </si>
-  <si>
-    <t>Pair of engraved bone dice</t>
-  </si>
-  <si>
-    <t>Painted gold child's sarcophagus</t>
-  </si>
-  <si>
-    <t>Jeweled anklet</t>
-  </si>
-  <si>
-    <t>Bottle stopper cork embossed with gold leaf and set with amethysts</t>
-  </si>
-  <si>
-    <t>Silk robe with gold embroidery</t>
-  </si>
-  <si>
-    <t>Copper chalice with silver filigree</t>
-  </si>
-  <si>
-    <t>Gold jewelry box with platinum filigree</t>
-  </si>
-  <si>
-    <t>Embroidered glove set with jewel chips</t>
-  </si>
-  <si>
-    <t>Gold dragon comb set with red garnets as eyes</t>
-  </si>
-  <si>
-    <t>Bronze crown</t>
-  </si>
-  <si>
-    <t>Black velvet mask stitched with silver thread</t>
-  </si>
-  <si>
-    <t>Gold cup set with emeralds</t>
-  </si>
-  <si>
-    <t>Platinum bracelet set with a sapphire</t>
-  </si>
-  <si>
-    <t>Small gold idol</t>
-  </si>
-  <si>
-    <t>Silver necklace with a gemstone pendant</t>
-  </si>
-  <si>
-    <t>Cloth-of-gold vestments</t>
-  </si>
-  <si>
-    <t>Small gold statuette set with rubies</t>
-  </si>
-  <si>
-    <t>Embroidered silk and velvet mantle set with numerous moonstones</t>
-  </si>
-  <si>
-    <t>Carved harp of exotic wood with ivory inlay and zircon gems</t>
-  </si>
-  <si>
-    <t>Large gold bracelet</t>
-  </si>
-  <si>
-    <t>Small gold bracelet</t>
-  </si>
-  <si>
-    <t>Jeweled platinum ring</t>
-  </si>
-  <si>
-    <t>Old masterpiece painting</t>
-  </si>
-  <si>
-    <t>Silver-plated steellongsword with jet set in hilt</t>
-  </si>
-  <si>
-    <t>Carved ivory statuette</t>
-  </si>
-  <si>
-    <t>Carved bone statuette</t>
-  </si>
-  <si>
-    <t>Jeweled gold crown</t>
-  </si>
-  <si>
-    <t>Fine gold chain set with a fire opal</t>
-  </si>
-  <si>
-    <t>Silver chalice set with moonstones</t>
-  </si>
-  <si>
-    <t>Gold ring set with bloodstones</t>
-  </si>
-  <si>
-    <t>Silver ewer</t>
-  </si>
-  <si>
-    <t>7500 GP</t>
-  </si>
-  <si>
-    <t>2500 GP</t>
-  </si>
-  <si>
-    <t>750 GP</t>
-  </si>
-  <si>
-    <t>250 GP</t>
-  </si>
-  <si>
-    <t>25 GP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1666,7 +1139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1674,51 +1147,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFDDDDDD"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFDDDDDD"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFDDDDDD"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFDDDDDD"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFDDDDDD"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2001,7 +1438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
@@ -2509,1700 +1946,6 @@
       <c r="A100" t="s">
         <v>7</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:B100"/>
-  <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="38" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A82" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A85" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A87" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A88" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A89" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A91" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A92" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:A12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="26.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>275</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:E35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.26953125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="22.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCBA4FC-9598-41EC-8C4E-7370B929C14F}">
-  <dimension ref="A1:E37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="69.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>476</v>
-      </c>
-      <c r="B1" t="s">
-        <v>475</v>
-      </c>
-      <c r="C1" t="s">
-        <v>474</v>
-      </c>
-      <c r="D1" t="s">
-        <v>473</v>
-      </c>
-      <c r="E1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>471</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>467</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>464</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>451</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>431</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="4"/>
-    </row>
-    <row r="29" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="30" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525A4CF5-6787-4E58-9D8C-73D86D0F6747}">
-  <dimension ref="A1:J28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>529</v>
-      </c>
-      <c r="B1" t="s">
-        <v>528</v>
-      </c>
-      <c r="C1" t="s">
-        <v>527</v>
-      </c>
-      <c r="D1" t="s">
-        <v>526</v>
-      </c>
-      <c r="E1" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>522</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>509</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>503</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>499</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>498</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>496</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>492</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>491</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>487</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>486</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>485</v>
-      </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6371,17 +4114,17 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>424</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>424</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>424</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -6521,12 +4264,12 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>425</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>425</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
@@ -6591,12 +4334,12 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>426</v>
+        <v>358</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>426</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
@@ -6869,17 +4612,17 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>427</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>427</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>427</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
@@ -7318,73 +5061,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7394,502 +5075,1021 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>351</v>
+        <v>337</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>352</v>
+        <v>338</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>353</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>354</v>
+        <v>340</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>357</v>
+        <v>343</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>358</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>367</v>
+        <v>353</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>369</v>
+        <v>355</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:B100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F107" sqref="F107"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed first draft of gem searching. updated readme with relevent info
</commit_message>
<xml_diff>
--- a/magic_item_tables.xlsx
+++ b/magic_item_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave_\Documents\DND tool\dnd_random_generation_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEFADC0-E0B7-424C-B932-FAE5CACE1D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD663345-9C6F-4784-8EF5-0FAD35DAC608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12990" yWindow="5010" windowWidth="20820" windowHeight="17410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12990" yWindow="3590" windowWidth="20820" windowHeight="17410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table A" sheetId="1" r:id="rId1"/>
@@ -1076,9 +1076,6 @@
     <t>Roll</t>
   </si>
   <si>
-    <t>Spell scroll: Cantrip</t>
-  </si>
-  <si>
     <t>scroll of protection</t>
   </si>
   <si>
@@ -1119,6 +1116,9 @@
   </si>
   <si>
     <t>Spell Scroll (Level 9)</t>
+  </si>
+  <si>
+    <t>Spell Scroll (Cantrip)</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1445,8 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51:G52"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1460,7 +1460,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1868,7 +1868,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1876,7 +1876,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1884,7 +1884,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1892,7 +1892,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1900,7 +1900,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1908,7 +1908,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1916,7 +1916,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1924,7 +1924,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1932,7 +1932,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1940,7 +1940,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -2028,7 +2028,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -2036,7 +2036,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -2044,7 +2044,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -2052,7 +2052,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -2060,7 +2060,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -2068,7 +2068,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -2076,7 +2076,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -2084,7 +2084,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -2092,7 +2092,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -2100,7 +2100,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -2108,7 +2108,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -2116,7 +2116,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -2124,7 +2124,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -2132,7 +2132,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -2140,7 +2140,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -2148,7 +2148,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -2156,7 +2156,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -2164,7 +2164,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -2172,7 +2172,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -2180,7 +2180,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -2188,7 +2188,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -2196,7 +2196,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -2204,7 +2204,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -2212,7 +2212,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -2288,7 +2288,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2728,7 +2728,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -2736,7 +2736,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -2744,7 +2744,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -2752,7 +2752,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -2760,7 +2760,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -2768,7 +2768,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -2776,7 +2776,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -2784,7 +2784,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -2792,7 +2792,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -2800,7 +2800,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -3116,7 +3116,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -3244,7 +3244,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -3252,7 +3252,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -3260,7 +3260,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -3268,7 +3268,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -3276,7 +3276,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -3284,7 +3284,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -3292,7 +3292,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -3660,7 +3660,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -3668,7 +3668,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -3676,7 +3676,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -3684,7 +3684,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -3692,7 +3692,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -3796,7 +3796,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -3804,7 +3804,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -3812,7 +3812,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -3944,7 +3944,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -4272,7 +4272,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -4280,7 +4280,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -4288,7 +4288,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -4296,7 +4296,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -4304,7 +4304,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -4312,7 +4312,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -4320,7 +4320,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -4328,7 +4328,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -4336,7 +4336,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -4344,7 +4344,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -4352,7 +4352,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -4360,7 +4360,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -4368,7 +4368,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -4376,7 +4376,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -4384,7 +4384,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -4392,7 +4392,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -4400,7 +4400,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -4648,7 +4648,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -4656,7 +4656,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -4664,7 +4664,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -4672,7 +4672,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -4680,7 +4680,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -4771,7 +4771,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -4779,7 +4779,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -4787,7 +4787,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -4795,7 +4795,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -4803,7 +4803,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -4811,7 +4811,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -4819,7 +4819,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -4827,7 +4827,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -4835,7 +4835,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -4843,7 +4843,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -4851,7 +4851,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -4859,7 +4859,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -4867,7 +4867,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -4875,7 +4875,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -4883,7 +4883,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -4891,7 +4891,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -4899,7 +4899,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -4907,7 +4907,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -4915,7 +4915,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -4923,7 +4923,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -4931,7 +4931,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -4939,7 +4939,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -4947,7 +4947,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -4955,7 +4955,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -4963,7 +4963,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -4971,7 +4971,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -4979,7 +4979,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -4987,7 +4987,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -4995,7 +4995,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -5003,7 +5003,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -5011,7 +5011,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -5339,7 +5339,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -5347,7 +5347,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -5355,7 +5355,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -5363,7 +5363,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -5371,7 +5371,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -5379,7 +5379,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -5387,7 +5387,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -5395,7 +5395,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -5403,7 +5403,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -5411,7 +5411,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -5419,7 +5419,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -5427,7 +5427,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -5435,7 +5435,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -5443,7 +5443,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -5451,7 +5451,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -5599,7 +5599,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -6427,7 +6427,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -6915,7 +6915,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -6987,7 +6987,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -7255,7 +7255,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -8083,7 +8083,7 @@
         <v>346</v>
       </c>
       <c r="B1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -8324,7 +8324,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -8332,7 +8332,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -8340,7 +8340,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>